<commit_message>
Fix: Error codigo ShipsManager
Referencia a un Vector3 eliminado.
</commit_message>
<xml_diff>
--- a/Kanban.xlsx
+++ b/Kanban.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Juegos Unity\Desperate Escape\FinalUnity_Coderhouse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871DF11D-E459-4C66-895C-E6360F73E258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43428506-479F-4538-B669-2550D24089A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="3" xr2:uid="{FC4DB9D1-58FC-4004-B030-7017194B0D1A}"/>
   </bookViews>
@@ -393,6 +393,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -403,18 +415,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -756,125 +756,125 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="16"/>
+      <c r="E2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="11" t="s">
+      <c r="F2" s="16"/>
+      <c r="G2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="12"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
         <v>1001</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="14"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>1002</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="16"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>1003</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="16"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="12"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>1004</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>1005</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="16"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="12"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>1006</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="16"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="12"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>1007</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="16"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="12"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>1008</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="16"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <v>1009</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="14"/>
     </row>
     <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -898,36 +898,36 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="G11:H11"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15" xr:uid="{74E52489-7F37-47B8-9662-FCE880C5CCAA}">
@@ -953,44 +953,44 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="16"/>
+      <c r="E2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="11" t="s">
+      <c r="F2" s="16"/>
+      <c r="G2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="12"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
         <v>2001</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="13" t="s">
+      <c r="C3" s="17"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="14"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>2002</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="16"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
@@ -1000,78 +1000,78 @@
         <v>11</v>
       </c>
       <c r="D5" s="20"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="16"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="12"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>2004</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>2005</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="16"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="12"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>2006</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="16"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="12"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>2007</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="16"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="12"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>2008</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="16"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <v>2009</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="14"/>
     </row>
     <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1095,36 +1095,36 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:H9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="G11:H11"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15" xr:uid="{E5397D40-FA7C-4FCA-B982-9D013F8A4377}">
@@ -1150,70 +1150,70 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="16"/>
+      <c r="E2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="11" t="s">
+      <c r="F2" s="16"/>
+      <c r="G2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="12"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="4">
         <v>3001</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="14"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>3002</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="16"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>3003</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="16"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="12"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>3004</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
@@ -1223,54 +1223,54 @@
         <v>16</v>
       </c>
       <c r="D7" s="20"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="16"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="12"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>3006</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="16"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="12"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>3007</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="16"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="12"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>3008</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="16"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <v>3009</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="14"/>
     </row>
     <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1294,6 +1294,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="G5:H5"/>
@@ -1310,20 +1324,6 @@
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15" xr:uid="{3DBB849A-A198-4409-B467-065D34973921}">
@@ -1345,6 +1345,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1352,44 +1353,44 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="16"/>
+      <c r="E2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="11" t="s">
+      <c r="F2" s="16"/>
+      <c r="G2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="12"/>
+      <c r="H2" s="16"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
         <v>4001</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="13" t="s">
+      <c r="C3" s="17"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="14"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>4002</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="16"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
@@ -1399,80 +1400,80 @@
         <v>19</v>
       </c>
       <c r="D5" s="20"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="16"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="12"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>4004</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="16"/>
+      <c r="H6" s="12"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>4005</v>
       </c>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="15" t="s">
+      <c r="C7" s="11"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="16"/>
+      <c r="H7" s="12"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>4006</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="16"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="12"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>4007</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="16"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="12"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>4008</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="16"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <v>4009</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="14"/>
       <c r="I11" s="8"/>
     </row>
     <row r="14" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1499,12 +1500,23 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="G7:H7"/>
@@ -1512,23 +1524,12 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="G8:H8"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C15" xr:uid="{0F64C707-0751-403C-9180-6F7A00DA5214}">

</xml_diff>